<commit_message>
Standard codes from UN OCHA and Special Codes
Tom Haythornthwaite update
</commit_message>
<xml_diff>
--- a/Data/GazetteerSqKm/MWIAdmin0GazJn.xlsx
+++ b/Data/GazetteerSqKm/MWIAdmin0GazJn.xlsx
@@ -106,67 +106,67 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>OBJECTID__</t>
+          <t>ADM0_EN</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Shape__</t>
+          <t>ADM0_PCODE</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>admin0Name_en</t>
+          <t>date</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>admin0Pcode</t>
+          <t>validOn</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>admin0RefName</t>
+          <t>validTo</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>admin0AltName1_en</t>
+          <t>OBJECTID</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>admin0AltName2_en</t>
+          <t>ADM0_EN_1</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>ADM0_PCODE_1</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>validOn</t>
+          <t>date_1</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>validTo</t>
+          <t>validOn_1</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
+          <t>validTo_1</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
           <t>Shape_Length</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Shape_Area</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>OBJECTID</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
@@ -179,61 +179,54 @@
       <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Malawi</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>MW</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>45014</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>45021</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>&lt;Null&gt;</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
         <v>1</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Polygon</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>Malawi</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>MW</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>&lt;Null&gt;</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>&lt;Null&gt;</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>&lt;Null&gt;</t>
-        </is>
-      </c>
-      <c r="I2" s="2" t="n">
-        <v>43346</v>
-      </c>
       <c r="J2" s="2" t="n">
-        <v>43389</v>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>&lt;Null&gt;</t>
-        </is>
-      </c>
-      <c r="L2" t="n">
-        <v>31.909743</v>
+        <v>45014</v>
+      </c>
+      <c r="K2" s="2" t="n">
+        <v>45021</v>
       </c>
       <c r="M2" t="n">
-        <v>8.001588</v>
+        <v>4321706.252511752</v>
       </c>
       <c r="N2" t="n">
-        <v>1</v>
+        <v>93271440920.29195</v>
       </c>
       <c r="O2" t="n">
-        <v>95777.6875</v>
+        <v>93271.44092029191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>